<commit_message>
Add arable rev to summarised bar plots
</commit_message>
<xml_diff>
--- a/CleanData/Guideline Creation/All Guidelines Sheet v2.xlsx
+++ b/CleanData/Guideline Creation/All Guidelines Sheet v2.xlsx
@@ -13260,4 +13260,247 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="RSPB Document" ma:contentTypeID="0x010100C277DC555996614A91CBD8E66D5843B400F00585E901B94A498EB29352A6A6478E" ma:contentTypeVersion="9" ma:contentTypeDescription="RSPB Document" ma:contentTypeScope="" ma:versionID="3a09cb41067aea0b3bcae64593430082">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5e7e1ee7-c46a-4dcb-b850-e1e58f5c63dc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="41b4f51899879990313be95609527478" ns2:_="">
+    <xsd:import namespace="5e7e1ee7-c46a-4dcb-b850-e1e58f5c63dc"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:Active_x002f_Inactive" minOccurs="0"/>
+                <xsd:element ref="ns2:k1641ee193934d5fb8c7d83caa06c3e2" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAllLabel" minOccurs="0"/>
+                <xsd:element ref="ns2:b72549223b3c4efea3869a351a81f6bb" minOccurs="0"/>
+                <xsd:element ref="ns2:d1bd46d554fb4aaf819291a18921284c" minOccurs="0"/>
+                <xsd:element ref="ns2:o5417782d7ac4612904fa4c8d48ab41e" minOccurs="0"/>
+                <xsd:element ref="ns2:k54ff54ece1a404cbcf4f781d58e442b" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="5e7e1ee7-c46a-4dcb-b850-e1e58f5c63dc" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="8" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{1abbb8c4-e483-4870-bac2-8a2966da0863}" ma:internalName="TaxCatchAll" ma:readOnly="false" ma:showField="CatchAllData" ma:web="5e7e1ee7-c46a-4dcb-b850-e1e58f5c63dc">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="Active_x002f_Inactive" ma:index="14" nillable="true" ma:displayName="Active?" ma:default="1" ma:internalName="Active_x002F_Inactive" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="k1641ee193934d5fb8c7d83caa06c3e2" ma:index="15" nillable="true" ma:taxonomy="true" ma:internalName="k1641ee193934d5fb8c7d83caa06c3e2" ma:taxonomyFieldName="Document_x0020_Type" ma:displayName="Document Type" ma:readOnly="false" ma:fieldId="{41641ee1-9393-4d5f-b8c7-d83caa06c3e2}" ma:sspId="39505d5b-8520-4033-8131-5c54fdfb80bd" ma:termSetId="811b141a-8675-4168-9805-15446faf0d14" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAllLabel" ma:index="16" nillable="true" ma:displayName="Taxonomy Catch All Column1" ma:hidden="true" ma:list="{1abbb8c4-e483-4870-bac2-8a2966da0863}" ma:internalName="TaxCatchAllLabel" ma:readOnly="false" ma:showField="CatchAllDataLabel" ma:web="5e7e1ee7-c46a-4dcb-b850-e1e58f5c63dc">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="b72549223b3c4efea3869a351a81f6bb" ma:index="17" nillable="true" ma:taxonomy="true" ma:internalName="b72549223b3c4efea3869a351a81f6bb" ma:taxonomyFieldName="Organisational_x0020_Unit" ma:displayName="Organisational Unit" ma:readOnly="false" ma:fieldId="{b7254922-3b3c-4efe-a386-9a351a81f6bb}" ma:sspId="39505d5b-8520-4033-8131-5c54fdfb80bd" ma:termSetId="489ebd6e-1d29-48bc-932a-d5a04d564a7e" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="d1bd46d554fb4aaf819291a18921284c" ma:index="18" nillable="true" ma:taxonomy="true" ma:internalName="d1bd46d554fb4aaf819291a18921284c" ma:taxonomyFieldName="RSPB_x0020_Location" ma:displayName="RSPB Location" ma:readOnly="false" ma:fieldId="{d1bd46d5-54fb-4aaf-8192-91a18921284c}" ma:sspId="39505d5b-8520-4033-8131-5c54fdfb80bd" ma:termSetId="3a999876-d616-45d8-ba34-cafd58b4ec09" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="o5417782d7ac4612904fa4c8d48ab41e" ma:index="19" nillable="true" ma:taxonomy="true" ma:internalName="o5417782d7ac4612904fa4c8d48ab41e" ma:taxonomyFieldName="Collection_x0020_Name" ma:displayName="Collection Name" ma:readOnly="false" ma:fieldId="{85417782-d7ac-4612-904f-a4c8d48ab41e}" ma:sspId="39505d5b-8520-4033-8131-5c54fdfb80bd" ma:termSetId="cbf41675-b644-4be8-bb76-870d4150a3d7" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="k54ff54ece1a404cbcf4f781d58e442b" ma:index="20" nillable="true" ma:taxonomy="true" ma:internalName="k54ff54ece1a404cbcf4f781d58e442b" ma:taxonomyFieldName="Security_x0020_Handling" ma:displayName="Security Handling" ma:readOnly="false" ma:default="1;#Internal Only|3727573c-2052-4b98-b369-5a376d94df50" ma:fieldId="{454ff54e-ce1a-404c-bcf4-f781d58e442b}" ma:sspId="39505d5b-8520-4033-8131-5c54fdfb80bd" ma:termSetId="2a1d6a0b-bbe9-4b7b-a023-7d4ecb920ea6" ma:anchorId="cf388454-8e58-4fec-a418-c767fd95ab9f" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <d1bd46d554fb4aaf819291a18921284c xmlns="5e7e1ee7-c46a-4dcb-b850-e1e58f5c63dc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </d1bd46d554fb4aaf819291a18921284c>
+    <Active_x002f_Inactive xmlns="5e7e1ee7-c46a-4dcb-b850-e1e58f5c63dc">true</Active_x002f_Inactive>
+    <o5417782d7ac4612904fa4c8d48ab41e xmlns="5e7e1ee7-c46a-4dcb-b850-e1e58f5c63dc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </o5417782d7ac4612904fa4c8d48ab41e>
+    <b72549223b3c4efea3869a351a81f6bb xmlns="5e7e1ee7-c46a-4dcb-b850-e1e58f5c63dc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b72549223b3c4efea3869a351a81f6bb>
+    <TaxCatchAll xmlns="5e7e1ee7-c46a-4dcb-b850-e1e58f5c63dc">
+      <Value>1</Value>
+    </TaxCatchAll>
+    <TaxCatchAllLabel xmlns="5e7e1ee7-c46a-4dcb-b850-e1e58f5c63dc" xsi:nil="true"/>
+    <k54ff54ece1a404cbcf4f781d58e442b xmlns="5e7e1ee7-c46a-4dcb-b850-e1e58f5c63dc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal Only</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">3727573c-2052-4b98-b369-5a376d94df50</TermId>
+        </TermInfo>
+      </Terms>
+    </k54ff54ece1a404cbcf4f781d58e442b>
+    <k1641ee193934d5fb8c7d83caa06c3e2 xmlns="5e7e1ee7-c46a-4dcb-b850-e1e58f5c63dc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </k1641ee193934d5fb8c7d83caa06c3e2>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD8E3BC-9EAC-4AB4-B5BD-6E925F5A63E5}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2E544B7-6CED-44F1-9C16-12D526C5EE49}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B815890-DFFC-4B9A-BAA6-CA34812DFE56}"/>
 </file>
</xml_diff>